<commit_message>
update van History, kleine update STAP vnw
</commit_message>
<xml_diff>
--- a/src/sastadev/data/methods/STAP_Index_Current.xlsx
+++ b/src/sastadev/data/methods/STAP_Index_Current.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/a3248526/git/sastadev_package/src/sastadev/data/methods/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dropbox\jodijk\myprograms\python\sastacode\mysastadev\src\sastadev\data\methods\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5C4612C-E497-C745-ACD2-B31EEBD3C6C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89E104CA-089E-4E05-9FD2-18C33EDA55BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="30240" windowHeight="19640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -518,17 +518,6 @@
 </t>
   </si>
   <si>
-    <t>//node[@pt="vnw" and 
-  not(@vwtype="bez") and
-    (@persoon="3"
-    or @persoon="3p"
-    or @persoon="3m"
-    or @persoon="3v"
-    or @persoon="3o")
-    and not(@pos="adv"
-        or @rel="det")]</t>
-  </si>
-  <si>
     <t>S019</t>
   </si>
   <si>
@@ -569,6 +558,20 @@
   </si>
   <si>
     <t>Literal</t>
+  </si>
+  <si>
+    <t>//node[@pt="vnw" and 
+  (not(@vwtype="bez") and
+    (@persoon="3"
+    or @persoon="3p"
+    or @persoon="3m"
+    or @persoon="3v"
+    or @persoon="3o")
+    and not(@pos="adv"
+        or @rel="det") and
+        @pdtype!="adv-pron") or
+  (@vwtype="aanw" and @positie="nom" and @pdtype!="adv-pron")        
+        ]</t>
   </si>
 </sst>
 </file>
@@ -1000,29 +1003,29 @@
   <dimension ref="A1:U148"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="5" ySplit="1" topLeftCell="J2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="5" ySplit="1" topLeftCell="J6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="P3" sqref="P3"/>
+      <selection pane="bottomRight" activeCell="K10" sqref="K10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="8.83203125" style="2"/>
-    <col min="2" max="2" width="18.1640625" style="2" customWidth="1"/>
+    <col min="1" max="1" width="8.77734375" style="2"/>
+    <col min="2" max="2" width="18.109375" style="2" customWidth="1"/>
     <col min="3" max="4" width="15" style="2" customWidth="1"/>
-    <col min="5" max="5" width="40.5" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="32.83203125" style="2" customWidth="1"/>
-    <col min="8" max="8" width="16.5" style="2" customWidth="1"/>
+    <col min="5" max="5" width="40.44140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="32.77734375" style="2" customWidth="1"/>
+    <col min="8" max="8" width="16.44140625" style="2" customWidth="1"/>
     <col min="9" max="9" width="12" style="2" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.5" style="2" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="61.5" style="7" customWidth="1"/>
-    <col min="13" max="20" width="8.83203125" style="2"/>
-    <col min="21" max="21" width="16.83203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="22" max="16384" width="8.83203125" style="2"/>
+    <col min="10" max="10" width="10.44140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="61.44140625" style="7" customWidth="1"/>
+    <col min="13" max="20" width="8.77734375" style="2"/>
+    <col min="21" max="21" width="16.77734375" style="2" bestFit="1" customWidth="1"/>
+    <col min="22" max="16384" width="8.77734375" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:21" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>8</v>
       </c>
@@ -1066,28 +1069,28 @@
         <v>104</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="P1" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="Q1" s="1" t="s">
         <v>150</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>151</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="S1" s="1" t="s">
         <v>152</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="T1" s="1" t="s">
         <v>153</v>
-      </c>
-      <c r="T1" s="1" t="s">
-        <v>154</v>
       </c>
       <c r="U1" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:21" ht="144" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:21" ht="144" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>37</v>
       </c>
@@ -1125,7 +1128,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="3" spans="1:21" ht="160" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:21" ht="144" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>38</v>
       </c>
@@ -1151,7 +1154,7 @@
         <v>97</v>
       </c>
       <c r="K3" s="6" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="L3" s="2" t="s">
         <v>98</v>
@@ -1163,7 +1166,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="4" spans="1:21" ht="32" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>39</v>
       </c>
@@ -1204,7 +1207,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="5" spans="1:21" ht="160" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:21" ht="144" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>40</v>
       </c>
@@ -1242,7 +1245,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>41</v>
       </c>
@@ -1280,7 +1283,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>42</v>
       </c>
@@ -1318,7 +1321,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="8" spans="1:21" ht="80" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:21" ht="72" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>43</v>
       </c>
@@ -1356,7 +1359,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="9" spans="1:21" ht="16" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>44</v>
       </c>
@@ -1397,7 +1400,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="10" spans="1:21" ht="144" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:21" ht="187.2" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>45</v>
       </c>
@@ -1426,7 +1429,7 @@
         <v>97</v>
       </c>
       <c r="K10" s="6" t="s">
-        <v>144</v>
+        <v>155</v>
       </c>
       <c r="L10" s="2" t="s">
         <v>98</v>
@@ -1438,7 +1441,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="11" spans="1:21" ht="16" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>46</v>
       </c>
@@ -1476,7 +1479,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="12" spans="1:21" ht="16" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
         <v>47</v>
       </c>
@@ -1514,7 +1517,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="13" spans="1:21" ht="16" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
         <v>48</v>
       </c>
@@ -1552,7 +1555,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="14" spans="1:21" ht="16" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
         <v>106</v>
       </c>
@@ -1590,7 +1593,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="15" spans="1:21" ht="16" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
         <v>110</v>
       </c>
@@ -1628,7 +1631,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="16" spans="1:21" ht="16" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
         <v>111</v>
       </c>
@@ -1666,7 +1669,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="17" spans="1:21" ht="32" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
         <v>112</v>
       </c>
@@ -1704,7 +1707,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="18" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
         <v>122</v>
       </c>
@@ -1742,7 +1745,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="19" spans="1:21" ht="32" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
         <v>123</v>
       </c>
@@ -1780,21 +1783,21 @@
         <v>135</v>
       </c>
     </row>
-    <row r="20" spans="1:21" ht="16" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="E20" s="2" t="s">
         <v>145</v>
       </c>
-      <c r="B20" s="2" t="s">
-        <v>148</v>
-      </c>
-      <c r="E20" s="2" t="s">
+      <c r="H20" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="K20" s="6" t="s">
         <v>146</v>
-      </c>
-      <c r="H20" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="K20" s="6" t="s">
-        <v>147</v>
       </c>
       <c r="L20" s="2" t="s">
         <v>98</v>
@@ -1803,315 +1806,315 @@
         <v>109</v>
       </c>
     </row>
-    <row r="24" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:21" x14ac:dyDescent="0.3">
       <c r="K24" s="6"/>
     </row>
-    <row r="25" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:21" x14ac:dyDescent="0.3">
       <c r="K25" s="6"/>
     </row>
-    <row r="26" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:21" x14ac:dyDescent="0.3">
       <c r="K26" s="6"/>
     </row>
-    <row r="27" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:21" x14ac:dyDescent="0.3">
       <c r="K27" s="6"/>
     </row>
-    <row r="28" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:21" x14ac:dyDescent="0.3">
       <c r="K28" s="6"/>
     </row>
-    <row r="29" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:21" x14ac:dyDescent="0.3">
       <c r="K29" s="6"/>
     </row>
-    <row r="30" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:21" x14ac:dyDescent="0.3">
       <c r="K30" s="6"/>
     </row>
-    <row r="31" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:21" x14ac:dyDescent="0.3">
       <c r="K31" s="6"/>
     </row>
-    <row r="32" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:21" x14ac:dyDescent="0.3">
       <c r="K32" s="6"/>
     </row>
-    <row r="33" spans="11:11" x14ac:dyDescent="0.2">
+    <row r="33" spans="11:11" x14ac:dyDescent="0.3">
       <c r="K33" s="6"/>
     </row>
-    <row r="34" spans="11:11" x14ac:dyDescent="0.2">
+    <row r="34" spans="11:11" x14ac:dyDescent="0.3">
       <c r="K34" s="6"/>
     </row>
-    <row r="35" spans="11:11" x14ac:dyDescent="0.2">
+    <row r="35" spans="11:11" x14ac:dyDescent="0.3">
       <c r="K35" s="6"/>
     </row>
-    <row r="36" spans="11:11" x14ac:dyDescent="0.2">
+    <row r="36" spans="11:11" x14ac:dyDescent="0.3">
       <c r="K36" s="6"/>
     </row>
-    <row r="37" spans="11:11" x14ac:dyDescent="0.2">
+    <row r="37" spans="11:11" x14ac:dyDescent="0.3">
       <c r="K37" s="6"/>
     </row>
-    <row r="38" spans="11:11" x14ac:dyDescent="0.2">
+    <row r="38" spans="11:11" x14ac:dyDescent="0.3">
       <c r="K38" s="6"/>
     </row>
-    <row r="39" spans="11:11" x14ac:dyDescent="0.2">
+    <row r="39" spans="11:11" x14ac:dyDescent="0.3">
       <c r="K39" s="6"/>
     </row>
-    <row r="40" spans="11:11" x14ac:dyDescent="0.2">
+    <row r="40" spans="11:11" x14ac:dyDescent="0.3">
       <c r="K40" s="6"/>
     </row>
-    <row r="43" spans="11:11" x14ac:dyDescent="0.2">
+    <row r="43" spans="11:11" x14ac:dyDescent="0.3">
       <c r="K43" s="6"/>
     </row>
-    <row r="44" spans="11:11" x14ac:dyDescent="0.2">
+    <row r="44" spans="11:11" x14ac:dyDescent="0.3">
       <c r="K44" s="6"/>
     </row>
-    <row r="45" spans="11:11" x14ac:dyDescent="0.2">
+    <row r="45" spans="11:11" x14ac:dyDescent="0.3">
       <c r="K45" s="6"/>
     </row>
-    <row r="46" spans="11:11" x14ac:dyDescent="0.2">
+    <row r="46" spans="11:11" x14ac:dyDescent="0.3">
       <c r="K46" s="6"/>
     </row>
-    <row r="47" spans="11:11" x14ac:dyDescent="0.2">
+    <row r="47" spans="11:11" x14ac:dyDescent="0.3">
       <c r="K47" s="6"/>
     </row>
-    <row r="48" spans="11:11" x14ac:dyDescent="0.2">
+    <row r="48" spans="11:11" x14ac:dyDescent="0.3">
       <c r="K48" s="6"/>
     </row>
-    <row r="49" spans="11:11" x14ac:dyDescent="0.2">
+    <row r="49" spans="11:11" x14ac:dyDescent="0.3">
       <c r="K49" s="6"/>
     </row>
-    <row r="50" spans="11:11" x14ac:dyDescent="0.2">
+    <row r="50" spans="11:11" x14ac:dyDescent="0.3">
       <c r="K50" s="6"/>
     </row>
-    <row r="51" spans="11:11" x14ac:dyDescent="0.2">
+    <row r="51" spans="11:11" x14ac:dyDescent="0.3">
       <c r="K51" s="6"/>
     </row>
-    <row r="52" spans="11:11" x14ac:dyDescent="0.2">
+    <row r="52" spans="11:11" x14ac:dyDescent="0.3">
       <c r="K52" s="6"/>
     </row>
-    <row r="53" spans="11:11" x14ac:dyDescent="0.2">
+    <row r="53" spans="11:11" x14ac:dyDescent="0.3">
       <c r="K53" s="6"/>
     </row>
-    <row r="55" spans="11:11" x14ac:dyDescent="0.2">
+    <row r="55" spans="11:11" x14ac:dyDescent="0.3">
       <c r="K55" s="6"/>
     </row>
-    <row r="56" spans="11:11" x14ac:dyDescent="0.2">
+    <row r="56" spans="11:11" x14ac:dyDescent="0.3">
       <c r="K56" s="6"/>
     </row>
-    <row r="57" spans="11:11" x14ac:dyDescent="0.2">
+    <row r="57" spans="11:11" x14ac:dyDescent="0.3">
       <c r="K57" s="6"/>
     </row>
-    <row r="58" spans="11:11" x14ac:dyDescent="0.2">
+    <row r="58" spans="11:11" x14ac:dyDescent="0.3">
       <c r="K58" s="6"/>
     </row>
-    <row r="59" spans="11:11" x14ac:dyDescent="0.2">
+    <row r="59" spans="11:11" x14ac:dyDescent="0.3">
       <c r="K59" s="6"/>
     </row>
-    <row r="60" spans="11:11" x14ac:dyDescent="0.2">
+    <row r="60" spans="11:11" x14ac:dyDescent="0.3">
       <c r="K60" s="6"/>
     </row>
-    <row r="62" spans="11:11" x14ac:dyDescent="0.2">
+    <row r="62" spans="11:11" x14ac:dyDescent="0.3">
       <c r="K62" s="6"/>
     </row>
-    <row r="63" spans="11:11" x14ac:dyDescent="0.2">
+    <row r="63" spans="11:11" x14ac:dyDescent="0.3">
       <c r="K63" s="6"/>
     </row>
-    <row r="64" spans="11:11" x14ac:dyDescent="0.2">
+    <row r="64" spans="11:11" x14ac:dyDescent="0.3">
       <c r="K64" s="6"/>
     </row>
-    <row r="65" spans="11:11" x14ac:dyDescent="0.2">
+    <row r="65" spans="11:11" x14ac:dyDescent="0.3">
       <c r="K65" s="6"/>
     </row>
-    <row r="66" spans="11:11" x14ac:dyDescent="0.2">
+    <row r="66" spans="11:11" x14ac:dyDescent="0.3">
       <c r="K66" s="6"/>
     </row>
-    <row r="68" spans="11:11" x14ac:dyDescent="0.2">
+    <row r="68" spans="11:11" x14ac:dyDescent="0.3">
       <c r="K68" s="6"/>
     </row>
-    <row r="69" spans="11:11" x14ac:dyDescent="0.2">
+    <row r="69" spans="11:11" x14ac:dyDescent="0.3">
       <c r="K69" s="6"/>
     </row>
-    <row r="71" spans="11:11" x14ac:dyDescent="0.2">
+    <row r="71" spans="11:11" x14ac:dyDescent="0.3">
       <c r="K71" s="6"/>
     </row>
-    <row r="72" spans="11:11" x14ac:dyDescent="0.2">
+    <row r="72" spans="11:11" x14ac:dyDescent="0.3">
       <c r="K72" s="6"/>
     </row>
-    <row r="73" spans="11:11" x14ac:dyDescent="0.2">
+    <row r="73" spans="11:11" x14ac:dyDescent="0.3">
       <c r="K73" s="6"/>
     </row>
-    <row r="74" spans="11:11" x14ac:dyDescent="0.2">
+    <row r="74" spans="11:11" x14ac:dyDescent="0.3">
       <c r="K74" s="6"/>
     </row>
-    <row r="75" spans="11:11" x14ac:dyDescent="0.2">
+    <row r="75" spans="11:11" x14ac:dyDescent="0.3">
       <c r="K75" s="6"/>
     </row>
-    <row r="76" spans="11:11" x14ac:dyDescent="0.2">
+    <row r="76" spans="11:11" x14ac:dyDescent="0.3">
       <c r="K76" s="6"/>
     </row>
-    <row r="77" spans="11:11" x14ac:dyDescent="0.2">
+    <row r="77" spans="11:11" x14ac:dyDescent="0.3">
       <c r="K77" s="6"/>
     </row>
-    <row r="78" spans="11:11" x14ac:dyDescent="0.2">
+    <row r="78" spans="11:11" x14ac:dyDescent="0.3">
       <c r="K78" s="6"/>
     </row>
-    <row r="79" spans="11:11" x14ac:dyDescent="0.2">
+    <row r="79" spans="11:11" x14ac:dyDescent="0.3">
       <c r="K79" s="6"/>
     </row>
-    <row r="80" spans="11:11" x14ac:dyDescent="0.2">
+    <row r="80" spans="11:11" x14ac:dyDescent="0.3">
       <c r="K80" s="6"/>
     </row>
-    <row r="81" spans="11:11" x14ac:dyDescent="0.2">
+    <row r="81" spans="11:11" x14ac:dyDescent="0.3">
       <c r="K81" s="6"/>
     </row>
-    <row r="82" spans="11:11" x14ac:dyDescent="0.2">
+    <row r="82" spans="11:11" x14ac:dyDescent="0.3">
       <c r="K82" s="6"/>
     </row>
-    <row r="83" spans="11:11" x14ac:dyDescent="0.2">
+    <row r="83" spans="11:11" x14ac:dyDescent="0.3">
       <c r="K83" s="6"/>
     </row>
-    <row r="84" spans="11:11" x14ac:dyDescent="0.2">
+    <row r="84" spans="11:11" x14ac:dyDescent="0.3">
       <c r="K84" s="6"/>
     </row>
-    <row r="85" spans="11:11" x14ac:dyDescent="0.2">
+    <row r="85" spans="11:11" x14ac:dyDescent="0.3">
       <c r="K85" s="6"/>
     </row>
-    <row r="87" spans="11:11" x14ac:dyDescent="0.2">
+    <row r="87" spans="11:11" x14ac:dyDescent="0.3">
       <c r="K87" s="6"/>
     </row>
-    <row r="88" spans="11:11" x14ac:dyDescent="0.2">
+    <row r="88" spans="11:11" x14ac:dyDescent="0.3">
       <c r="K88" s="6"/>
     </row>
-    <row r="89" spans="11:11" x14ac:dyDescent="0.2">
+    <row r="89" spans="11:11" x14ac:dyDescent="0.3">
       <c r="K89" s="6"/>
     </row>
-    <row r="90" spans="11:11" x14ac:dyDescent="0.2">
+    <row r="90" spans="11:11" x14ac:dyDescent="0.3">
       <c r="K90" s="6"/>
     </row>
-    <row r="91" spans="11:11" x14ac:dyDescent="0.2">
+    <row r="91" spans="11:11" x14ac:dyDescent="0.3">
       <c r="K91" s="6"/>
     </row>
-    <row r="92" spans="11:11" x14ac:dyDescent="0.2">
+    <row r="92" spans="11:11" x14ac:dyDescent="0.3">
       <c r="K92" s="6"/>
     </row>
-    <row r="94" spans="11:11" x14ac:dyDescent="0.2">
+    <row r="94" spans="11:11" x14ac:dyDescent="0.3">
       <c r="K94" s="6"/>
     </row>
-    <row r="95" spans="11:11" x14ac:dyDescent="0.2">
+    <row r="95" spans="11:11" x14ac:dyDescent="0.3">
       <c r="K95" s="6"/>
     </row>
-    <row r="96" spans="11:11" x14ac:dyDescent="0.2">
+    <row r="96" spans="11:11" x14ac:dyDescent="0.3">
       <c r="K96" s="6"/>
     </row>
-    <row r="99" spans="11:11" x14ac:dyDescent="0.2">
+    <row r="99" spans="11:11" x14ac:dyDescent="0.3">
       <c r="K99" s="6"/>
     </row>
-    <row r="100" spans="11:11" x14ac:dyDescent="0.2">
+    <row r="100" spans="11:11" x14ac:dyDescent="0.3">
       <c r="K100" s="6"/>
     </row>
-    <row r="101" spans="11:11" x14ac:dyDescent="0.2">
+    <row r="101" spans="11:11" x14ac:dyDescent="0.3">
       <c r="K101" s="6"/>
     </row>
-    <row r="102" spans="11:11" x14ac:dyDescent="0.2">
+    <row r="102" spans="11:11" x14ac:dyDescent="0.3">
       <c r="K102" s="6"/>
     </row>
-    <row r="103" spans="11:11" x14ac:dyDescent="0.2">
+    <row r="103" spans="11:11" x14ac:dyDescent="0.3">
       <c r="K103" s="6"/>
     </row>
-    <row r="106" spans="11:11" x14ac:dyDescent="0.2">
+    <row r="106" spans="11:11" x14ac:dyDescent="0.3">
       <c r="K106" s="6"/>
     </row>
-    <row r="107" spans="11:11" x14ac:dyDescent="0.2">
+    <row r="107" spans="11:11" x14ac:dyDescent="0.3">
       <c r="K107" s="6"/>
     </row>
-    <row r="112" spans="11:11" x14ac:dyDescent="0.2">
+    <row r="112" spans="11:11" x14ac:dyDescent="0.3">
       <c r="K112" s="6"/>
     </row>
-    <row r="113" spans="11:11" x14ac:dyDescent="0.2">
+    <row r="113" spans="11:11" x14ac:dyDescent="0.3">
       <c r="K113" s="6"/>
     </row>
-    <row r="114" spans="11:11" x14ac:dyDescent="0.2">
+    <row r="114" spans="11:11" x14ac:dyDescent="0.3">
       <c r="K114" s="6"/>
     </row>
-    <row r="115" spans="11:11" x14ac:dyDescent="0.2">
+    <row r="115" spans="11:11" x14ac:dyDescent="0.3">
       <c r="K115" s="8"/>
     </row>
-    <row r="116" spans="11:11" x14ac:dyDescent="0.2">
+    <row r="116" spans="11:11" x14ac:dyDescent="0.3">
       <c r="K116" s="6"/>
     </row>
-    <row r="117" spans="11:11" x14ac:dyDescent="0.2">
+    <row r="117" spans="11:11" x14ac:dyDescent="0.3">
       <c r="K117" s="6"/>
     </row>
-    <row r="118" spans="11:11" x14ac:dyDescent="0.2">
+    <row r="118" spans="11:11" x14ac:dyDescent="0.3">
       <c r="K118" s="6"/>
     </row>
-    <row r="119" spans="11:11" x14ac:dyDescent="0.2">
+    <row r="119" spans="11:11" x14ac:dyDescent="0.3">
       <c r="K119" s="6"/>
     </row>
-    <row r="120" spans="11:11" x14ac:dyDescent="0.2">
+    <row r="120" spans="11:11" x14ac:dyDescent="0.3">
       <c r="K120" s="6"/>
     </row>
-    <row r="121" spans="11:11" x14ac:dyDescent="0.2">
+    <row r="121" spans="11:11" x14ac:dyDescent="0.3">
       <c r="K121" s="6"/>
     </row>
-    <row r="122" spans="11:11" x14ac:dyDescent="0.2">
+    <row r="122" spans="11:11" x14ac:dyDescent="0.3">
       <c r="K122" s="6"/>
     </row>
-    <row r="126" spans="11:11" x14ac:dyDescent="0.2">
+    <row r="126" spans="11:11" x14ac:dyDescent="0.3">
       <c r="K126" s="6"/>
     </row>
-    <row r="127" spans="11:11" x14ac:dyDescent="0.2">
+    <row r="127" spans="11:11" x14ac:dyDescent="0.3">
       <c r="K127" s="6"/>
     </row>
-    <row r="128" spans="11:11" x14ac:dyDescent="0.2">
+    <row r="128" spans="11:11" x14ac:dyDescent="0.3">
       <c r="K128" s="6"/>
     </row>
-    <row r="129" spans="5:11" x14ac:dyDescent="0.2">
+    <row r="129" spans="5:11" x14ac:dyDescent="0.3">
       <c r="K129" s="6"/>
     </row>
-    <row r="130" spans="5:11" x14ac:dyDescent="0.2">
+    <row r="130" spans="5:11" x14ac:dyDescent="0.3">
       <c r="K130" s="6"/>
     </row>
-    <row r="131" spans="5:11" x14ac:dyDescent="0.2">
+    <row r="131" spans="5:11" x14ac:dyDescent="0.3">
       <c r="K131" s="6"/>
     </row>
-    <row r="132" spans="5:11" x14ac:dyDescent="0.2">
+    <row r="132" spans="5:11" x14ac:dyDescent="0.3">
       <c r="K132" s="6"/>
     </row>
-    <row r="133" spans="5:11" x14ac:dyDescent="0.2">
+    <row r="133" spans="5:11" x14ac:dyDescent="0.3">
       <c r="K133" s="6"/>
     </row>
-    <row r="134" spans="5:11" x14ac:dyDescent="0.2">
+    <row r="134" spans="5:11" x14ac:dyDescent="0.3">
       <c r="K134" s="6"/>
     </row>
-    <row r="135" spans="5:11" x14ac:dyDescent="0.2">
+    <row r="135" spans="5:11" x14ac:dyDescent="0.3">
       <c r="K135" s="6"/>
     </row>
-    <row r="136" spans="5:11" x14ac:dyDescent="0.2">
+    <row r="136" spans="5:11" x14ac:dyDescent="0.3">
       <c r="K136" s="6"/>
     </row>
-    <row r="137" spans="5:11" x14ac:dyDescent="0.2">
+    <row r="137" spans="5:11" x14ac:dyDescent="0.3">
       <c r="K137" s="6"/>
     </row>
-    <row r="138" spans="5:11" x14ac:dyDescent="0.2">
+    <row r="138" spans="5:11" x14ac:dyDescent="0.3">
       <c r="E138" s="3"/>
       <c r="K138" s="6"/>
     </row>
-    <row r="139" spans="5:11" x14ac:dyDescent="0.2">
+    <row r="139" spans="5:11" x14ac:dyDescent="0.3">
       <c r="E139" s="3"/>
     </row>
-    <row r="140" spans="5:11" x14ac:dyDescent="0.2">
+    <row r="140" spans="5:11" x14ac:dyDescent="0.3">
       <c r="E140" s="4"/>
       <c r="K140" s="6"/>
     </row>
-    <row r="142" spans="5:11" x14ac:dyDescent="0.2">
+    <row r="142" spans="5:11" x14ac:dyDescent="0.3">
       <c r="K142" s="6"/>
     </row>
-    <row r="144" spans="5:11" x14ac:dyDescent="0.2">
+    <row r="144" spans="5:11" x14ac:dyDescent="0.3">
       <c r="K144" s="6"/>
     </row>
-    <row r="146" spans="11:11" x14ac:dyDescent="0.2">
+    <row r="146" spans="11:11" x14ac:dyDescent="0.3">
       <c r="K146" s="6"/>
     </row>
-    <row r="147" spans="11:11" x14ac:dyDescent="0.2">
+    <row r="147" spans="11:11" x14ac:dyDescent="0.3">
       <c r="K147" s="6"/>
     </row>
-    <row r="148" spans="11:11" x14ac:dyDescent="0.2">
+    <row r="148" spans="11:11" x14ac:dyDescent="0.3">
       <c r="K148" s="6"/>
     </row>
   </sheetData>
@@ -2133,14 +2136,14 @@
       <selection activeCell="L14" sqref="L14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="22.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="2" customWidth="1"/>
-    <col min="12" max="12" width="25.5" customWidth="1"/>
+    <col min="12" max="12" width="25.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:12" ht="80" x14ac:dyDescent="0.2">
+    <row r="2" spans="2:12" ht="72" x14ac:dyDescent="0.3">
       <c r="B2" t="s">
         <v>22</v>
       </c>
@@ -2157,12 +2160,12 @@
         <v>34</v>
       </c>
     </row>
-    <row r="3" spans="2:12" x14ac:dyDescent="0.2">
+    <row r="3" spans="2:12" x14ac:dyDescent="0.3">
       <c r="E3" s="10" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="2:12" ht="32" x14ac:dyDescent="0.2">
+    <row r="4" spans="2:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="C4" t="s">
         <v>16</v>
       </c>
@@ -2176,7 +2179,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="5" spans="2:12" x14ac:dyDescent="0.2">
+    <row r="5" spans="2:12" x14ac:dyDescent="0.3">
       <c r="E5" s="10" t="s">
         <v>19</v>
       </c>
@@ -2187,7 +2190,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="7" spans="2:12" ht="48" x14ac:dyDescent="0.2">
+    <row r="7" spans="2:12" ht="57.6" x14ac:dyDescent="0.3">
       <c r="B7" t="s">
         <v>23</v>
       </c>
@@ -2205,11 +2208,11 @@
         <v>31</v>
       </c>
     </row>
-    <row r="8" spans="2:12" x14ac:dyDescent="0.2">
+    <row r="8" spans="2:12" x14ac:dyDescent="0.3">
       <c r="D8" s="9"/>
       <c r="E8" s="10"/>
     </row>
-    <row r="9" spans="2:12" x14ac:dyDescent="0.2">
+    <row r="9" spans="2:12" x14ac:dyDescent="0.3">
       <c r="C9" t="s">
         <v>26</v>
       </c>
@@ -2218,7 +2221,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="10" spans="2:12" ht="80" x14ac:dyDescent="0.2">
+    <row r="10" spans="2:12" ht="72" x14ac:dyDescent="0.3">
       <c r="D10" s="9"/>
       <c r="E10" s="10" t="s">
         <v>25</v>
@@ -2230,11 +2233,11 @@
         <v>33</v>
       </c>
     </row>
-    <row r="11" spans="2:12" x14ac:dyDescent="0.2">
+    <row r="11" spans="2:12" x14ac:dyDescent="0.3">
       <c r="D11" s="9"/>
       <c r="E11" s="10"/>
     </row>
-    <row r="12" spans="2:12" ht="80" x14ac:dyDescent="0.2">
+    <row r="12" spans="2:12" ht="72" x14ac:dyDescent="0.3">
       <c r="C12" t="s">
         <v>30</v>
       </c>
@@ -2246,11 +2249,11 @@
         <v>32</v>
       </c>
     </row>
-    <row r="13" spans="2:12" x14ac:dyDescent="0.2">
+    <row r="13" spans="2:12" x14ac:dyDescent="0.3">
       <c r="D13" s="9"/>
       <c r="E13" s="10"/>
     </row>
-    <row r="14" spans="2:12" ht="304" x14ac:dyDescent="0.2">
+    <row r="14" spans="2:12" ht="288" x14ac:dyDescent="0.3">
       <c r="C14" t="s">
         <v>7</v>
       </c>
@@ -2260,51 +2263,51 @@
         <v>36</v>
       </c>
     </row>
-    <row r="15" spans="2:12" x14ac:dyDescent="0.2">
+    <row r="15" spans="2:12" x14ac:dyDescent="0.3">
       <c r="D15" s="9"/>
       <c r="E15" s="10"/>
     </row>
-    <row r="16" spans="2:12" x14ac:dyDescent="0.2">
+    <row r="16" spans="2:12" x14ac:dyDescent="0.3">
       <c r="D16" s="9"/>
       <c r="E16" s="10"/>
     </row>
-    <row r="17" spans="4:5" x14ac:dyDescent="0.2">
+    <row r="17" spans="4:5" x14ac:dyDescent="0.3">
       <c r="D17" s="9"/>
       <c r="E17" s="10"/>
     </row>
-    <row r="18" spans="4:5" x14ac:dyDescent="0.2">
+    <row r="18" spans="4:5" x14ac:dyDescent="0.3">
       <c r="D18" s="9"/>
       <c r="E18" s="10"/>
     </row>
-    <row r="19" spans="4:5" x14ac:dyDescent="0.2">
+    <row r="19" spans="4:5" x14ac:dyDescent="0.3">
       <c r="D19" s="9"/>
       <c r="E19" s="10"/>
     </row>
-    <row r="20" spans="4:5" x14ac:dyDescent="0.2">
+    <row r="20" spans="4:5" x14ac:dyDescent="0.3">
       <c r="D20" s="9"/>
       <c r="E20" s="10"/>
     </row>
-    <row r="21" spans="4:5" x14ac:dyDescent="0.2">
+    <row r="21" spans="4:5" x14ac:dyDescent="0.3">
       <c r="D21" s="9"/>
       <c r="E21" s="10"/>
     </row>
-    <row r="22" spans="4:5" x14ac:dyDescent="0.2">
+    <row r="22" spans="4:5" x14ac:dyDescent="0.3">
       <c r="D22" s="9"/>
       <c r="E22" s="10"/>
     </row>
-    <row r="23" spans="4:5" x14ac:dyDescent="0.2">
+    <row r="23" spans="4:5" x14ac:dyDescent="0.3">
       <c r="D23" s="9"/>
       <c r="E23" s="10"/>
     </row>
-    <row r="24" spans="4:5" x14ac:dyDescent="0.2">
+    <row r="24" spans="4:5" x14ac:dyDescent="0.3">
       <c r="D24" s="9"/>
       <c r="E24" s="10"/>
     </row>
-    <row r="25" spans="4:5" x14ac:dyDescent="0.2">
+    <row r="25" spans="4:5" x14ac:dyDescent="0.3">
       <c r="D25" s="9"/>
       <c r="E25" s="10"/>
     </row>
-    <row r="26" spans="4:5" x14ac:dyDescent="0.2">
+    <row r="26" spans="4:5" x14ac:dyDescent="0.3">
       <c r="D26" s="9"/>
       <c r="E26" s="10"/>
     </row>

</xml_diff>